<commit_message>
Analysis of results for WordSearch Analysis, explaining the figures, corroborating the hypothesis
</commit_message>
<xml_diff>
--- a/WordSearch.xlsx
+++ b/WordSearch.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1110,10 +1110,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U206"/>
+  <dimension ref="A1:U210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="G212" sqref="G212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -3710,44 +3710,48 @@
         <v>69.320843091334893</v>
       </c>
     </row>
-    <row r="162" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="4" t="s">
-        <v>187</v>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A161" s="6"/>
+      <c r="D161" s="6"/>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A162" s="3" t="s">
+        <v>235</v>
       </c>
       <c r="B162" s="3">
-        <v>110</v>
+        <v>829</v>
       </c>
       <c r="C162" s="3">
-        <v>7</v>
+        <v>480</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>188</v>
+        <v>236</v>
       </c>
       <c r="E162" s="3">
-        <v>26</v>
+        <v>487</v>
       </c>
       <c r="F162" s="3">
-        <v>0</v>
+        <v>319</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
-        <v>189</v>
+        <v>237</v>
       </c>
       <c r="B163" s="3">
-        <v>0</v>
+        <v>486</v>
       </c>
       <c r="C163" s="3">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>190</v>
+        <v>238</v>
       </c>
       <c r="E163" s="3">
-        <v>0</v>
+        <v>1473</v>
       </c>
       <c r="F163" s="3">
-        <v>0</v>
+        <v>36</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.25">
@@ -3755,50 +3759,50 @@
         <v>13</v>
       </c>
       <c r="B164" s="3">
+        <v>1315</v>
+      </c>
+      <c r="C164" s="3">
+        <v>498</v>
+      </c>
+      <c r="D164" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E164" s="3">
+        <v>1960</v>
+      </c>
+      <c r="F164" s="3">
+        <v>355</v>
+      </c>
+      <c r="G164" s="3">
+        <v>59.847328244274813</v>
+      </c>
+      <c r="H164" s="3">
+        <v>41.617819460726849</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A166" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B166" s="3">
         <v>110</v>
       </c>
-      <c r="C164" s="3">
+      <c r="C166" s="3">
         <v>7</v>
       </c>
-      <c r="D164" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E164" s="3">
+      <c r="D166" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="E166" s="3">
         <v>26</v>
       </c>
-      <c r="F164" s="3">
-        <v>0</v>
-      </c>
-      <c r="G164" s="3">
-        <v>19.117647058823529</v>
-      </c>
-      <c r="H164" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="166" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="B166" s="3">
-        <v>13</v>
-      </c>
-      <c r="C166" s="3">
-        <v>5</v>
-      </c>
-      <c r="D166" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="E166" s="3">
-        <v>369</v>
-      </c>
       <c r="F166" s="3">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B167" s="3">
         <v>0</v>
@@ -3807,7 +3811,7 @@
         <v>0</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E167" s="3">
         <v>0</v>
@@ -3821,233 +3825,233 @@
         <v>13</v>
       </c>
       <c r="B168" s="3">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="C168" s="3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D168" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E168" s="3">
-        <v>369</v>
+        <v>26</v>
       </c>
       <c r="F168" s="3">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G168" s="3">
-        <v>96.596858638743456</v>
+        <v>19.117647058823529</v>
       </c>
       <c r="H168" s="3">
-        <v>76.19047619047619</v>
+        <v>0</v>
       </c>
     </row>
     <row r="170" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B170" s="3">
+        <v>13</v>
+      </c>
+      <c r="C170" s="3">
+        <v>5</v>
+      </c>
+      <c r="D170" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="E170" s="3">
+        <v>369</v>
+      </c>
+      <c r="F170" s="3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A171" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B171" s="3">
+        <v>0</v>
+      </c>
+      <c r="C171" s="3">
+        <v>0</v>
+      </c>
+      <c r="D171" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E171" s="3">
+        <v>0</v>
+      </c>
+      <c r="F171" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A172" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B172" s="3">
+        <v>13</v>
+      </c>
+      <c r="C172" s="3">
+        <v>5</v>
+      </c>
+      <c r="D172" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E172" s="3">
+        <v>369</v>
+      </c>
+      <c r="F172" s="3">
+        <v>16</v>
+      </c>
+      <c r="G172" s="3">
+        <v>96.596858638743456</v>
+      </c>
+      <c r="H172" s="3">
+        <v>76.19047619047619</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A174" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="B170" s="3">
+      <c r="B174" s="3">
         <v>8</v>
       </c>
-      <c r="C170" s="3">
+      <c r="C174" s="3">
         <v>12</v>
       </c>
-      <c r="D170" s="3" t="s">
+      <c r="D174" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="E170" s="3">
+      <c r="E174" s="3">
         <v>577</v>
       </c>
-      <c r="F170" s="3">
+      <c r="F174" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="171" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A171" s="3" t="s">
+    <row r="175" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A175" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="B171" s="3">
+      <c r="B175" s="3">
         <v>151</v>
       </c>
-      <c r="C171" s="3">
+      <c r="C175" s="3">
         <v>20</v>
       </c>
-      <c r="D171" s="3" t="s">
+      <c r="D175" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="E171" s="3">
+      <c r="E175" s="3">
         <v>2934</v>
       </c>
-      <c r="F171" s="3">
+      <c r="F175" s="3">
         <v>113</v>
       </c>
     </row>
-    <row r="172" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A172" s="3" t="s">
+    <row r="176" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A176" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="B172" s="3">
+      <c r="B176" s="3">
         <v>186</v>
       </c>
-      <c r="C172" s="3">
+      <c r="C176" s="3">
         <v>76</v>
       </c>
-      <c r="D172" s="3" t="s">
+      <c r="D176" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="E172" s="3">
+      <c r="E176" s="3">
         <v>480</v>
       </c>
-      <c r="F172" s="3">
+      <c r="F176" s="3">
         <v>19</v>
       </c>
     </row>
-    <row r="173" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A173" s="3" t="s">
+    <row r="177" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A177" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="B173" s="3">
-        <v>0</v>
-      </c>
-      <c r="C173" s="3">
-        <v>0</v>
-      </c>
-      <c r="D173" s="3" t="s">
+      <c r="B177" s="3">
+        <v>0</v>
+      </c>
+      <c r="C177" s="3">
+        <v>0</v>
+      </c>
+      <c r="D177" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="E173" s="3">
+      <c r="E177" s="3">
         <v>94</v>
       </c>
-      <c r="F173" s="3">
+      <c r="F177" s="3">
         <v>29</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A174" s="3" t="s">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A178" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="B174" s="3">
-        <v>0</v>
-      </c>
-      <c r="C174" s="3">
-        <v>0</v>
-      </c>
-      <c r="D174" s="3" t="s">
+      <c r="B178" s="3">
+        <v>0</v>
+      </c>
+      <c r="C178" s="3">
+        <v>0</v>
+      </c>
+      <c r="D178" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="E174" s="3">
+      <c r="E178" s="3">
         <v>20</v>
       </c>
-      <c r="F174" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A175" s="3" t="s">
+      <c r="F178" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A179" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="B175" s="3">
+      <c r="B179" s="3">
         <v>11</v>
       </c>
-      <c r="C175" s="3">
+      <c r="C179" s="3">
         <v>1</v>
       </c>
-      <c r="D175" s="3" t="s">
+      <c r="D179" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="E175" s="3">
+      <c r="E179" s="3">
         <v>36</v>
       </c>
-      <c r="F175" s="3">
+      <c r="F179" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D176" s="3" t="s">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D180" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="E176" s="3">
+      <c r="E180" s="3">
         <v>3</v>
       </c>
-      <c r="F176" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D177" s="3" t="s">
+      <c r="F180" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D181" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="E177" s="3">
-        <v>13</v>
-      </c>
-      <c r="F177" s="3">
+      <c r="E181" s="3">
+        <v>13</v>
+      </c>
+      <c r="F181" s="3">
         <v>22</v>
-      </c>
-    </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A178" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B178" s="3">
-        <v>356</v>
-      </c>
-      <c r="C178" s="3">
-        <v>109</v>
-      </c>
-      <c r="D178" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E178" s="3">
-        <v>4157</v>
-      </c>
-      <c r="F178" s="3">
-        <v>195</v>
-      </c>
-      <c r="G178" s="3">
-        <v>92.111677376467981</v>
-      </c>
-      <c r="H178" s="3">
-        <v>64.14473684210526</v>
-      </c>
-    </row>
-    <row r="180" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A180" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="B180" s="3">
-        <v>2584</v>
-      </c>
-      <c r="C180" s="3">
-        <v>224</v>
-      </c>
-      <c r="D180" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="E180" s="3">
-        <v>2896</v>
-      </c>
-      <c r="F180" s="3">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A181" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="B181" s="3">
-        <v>0</v>
-      </c>
-      <c r="C181" s="3">
-        <v>0</v>
-      </c>
-      <c r="D181" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="E181" s="3">
-        <v>50</v>
-      </c>
-      <c r="F181" s="3">
-        <v>10</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.25">
@@ -4055,369 +4059,369 @@
         <v>13</v>
       </c>
       <c r="B182" s="3">
-        <v>2584</v>
+        <v>356</v>
       </c>
       <c r="C182" s="3">
-        <v>224</v>
+        <v>109</v>
       </c>
       <c r="D182" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E182" s="3">
-        <v>2946</v>
+        <v>4157</v>
       </c>
       <c r="F182" s="3">
-        <v>244</v>
+        <v>195</v>
       </c>
       <c r="G182" s="3">
-        <v>53.273056057866192</v>
+        <v>92.111677376467981</v>
       </c>
       <c r="H182" s="3">
-        <v>52.136752136752143</v>
+        <v>64.14473684210526</v>
       </c>
     </row>
     <row r="184" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="3" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B184" s="3">
-        <v>282</v>
+        <v>2584</v>
       </c>
       <c r="C184" s="3">
-        <v>846</v>
+        <v>224</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E184" s="3">
-        <v>728</v>
+        <v>2896</v>
       </c>
       <c r="F184" s="3">
-        <v>247</v>
+        <v>234</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B185" s="3">
+        <v>0</v>
+      </c>
+      <c r="C185" s="3">
+        <v>0</v>
+      </c>
+      <c r="D185" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E185" s="3">
+        <v>50</v>
+      </c>
+      <c r="F185" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A186" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B186" s="3">
+        <v>2584</v>
+      </c>
+      <c r="C186" s="3">
+        <v>224</v>
+      </c>
+      <c r="D186" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E186" s="3">
+        <v>2946</v>
+      </c>
+      <c r="F186" s="3">
+        <v>244</v>
+      </c>
+      <c r="G186" s="3">
+        <v>53.273056057866192</v>
+      </c>
+      <c r="H186" s="3">
+        <v>52.136752136752143</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A188" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B188" s="3">
+        <v>282</v>
+      </c>
+      <c r="C188" s="3">
+        <v>846</v>
+      </c>
+      <c r="D188" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="E188" s="3">
+        <v>728</v>
+      </c>
+      <c r="F188" s="3">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A189" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="B185" s="3">
-        <v>0</v>
-      </c>
-      <c r="C185" s="3">
-        <v>0</v>
-      </c>
-      <c r="D185" s="3" t="s">
+      <c r="B189" s="3">
+        <v>0</v>
+      </c>
+      <c r="C189" s="3">
+        <v>0</v>
+      </c>
+      <c r="D189" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="E185" s="3">
+      <c r="E189" s="3">
         <v>6</v>
       </c>
-      <c r="F185" s="3">
+      <c r="F189" s="3">
         <v>16</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D186" s="3" t="s">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D190" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="E186" s="3">
-        <v>0</v>
-      </c>
-      <c r="F186" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A187" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B187" s="3">
+      <c r="E190" s="3">
+        <v>0</v>
+      </c>
+      <c r="F190" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A191" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B191" s="3">
         <v>282</v>
       </c>
-      <c r="C187" s="3">
+      <c r="C191" s="3">
         <v>846</v>
       </c>
-      <c r="D187" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E187" s="3">
+      <c r="D191" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E191" s="3">
         <v>734</v>
       </c>
-      <c r="F187" s="3">
+      <c r="F191" s="3">
         <v>263</v>
       </c>
-      <c r="G187" s="3">
+      <c r="G191" s="3">
         <v>72.244094488188978</v>
       </c>
-      <c r="H187" s="3">
+      <c r="H191" s="3">
         <v>23.715058611361592</v>
       </c>
     </row>
-    <row r="189" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A189" s="4" t="s">
+    <row r="193" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A193" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="B189" s="3">
+      <c r="B193" s="3">
         <v>2855</v>
       </c>
-      <c r="C189" s="3">
-        <v>13</v>
-      </c>
-      <c r="D189" s="3" t="s">
+      <c r="C193" s="3">
+        <v>13</v>
+      </c>
+      <c r="D193" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="E189" s="3">
+      <c r="E193" s="3">
         <v>28</v>
       </c>
-      <c r="F189" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="190" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A190" s="3" t="s">
+      <c r="F193" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A194" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="B190" s="3">
+      <c r="B194" s="3">
         <v>43</v>
       </c>
-      <c r="C190" s="3">
+      <c r="C194" s="3">
         <v>9</v>
       </c>
-      <c r="D190" s="3" t="s">
+      <c r="D194" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="E190" s="3">
+      <c r="E194" s="3">
         <v>143</v>
       </c>
-      <c r="F190" s="3">
+      <c r="F194" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="191" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A191" s="3" t="s">
+    <row r="195" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A195" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="B191" s="3">
-        <v>0</v>
-      </c>
-      <c r="C191" s="3">
-        <v>0</v>
-      </c>
-      <c r="D191" s="3" t="s">
+      <c r="B195" s="3">
+        <v>0</v>
+      </c>
+      <c r="C195" s="3">
+        <v>0</v>
+      </c>
+      <c r="D195" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="E191" s="3">
+      <c r="E195" s="3">
         <v>14</v>
       </c>
-      <c r="F191" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="192" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A192" s="3" t="s">
+      <c r="F195" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A196" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="B192" s="3">
-        <v>0</v>
-      </c>
-      <c r="C192" s="3">
-        <v>0</v>
-      </c>
-      <c r="D192" s="3" t="s">
+      <c r="B196" s="3">
+        <v>0</v>
+      </c>
+      <c r="C196" s="3">
+        <v>0</v>
+      </c>
+      <c r="D196" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="E192" s="3">
-        <v>0</v>
-      </c>
-      <c r="F192" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D193" s="3" t="s">
+      <c r="E196" s="3">
+        <v>0</v>
+      </c>
+      <c r="F196" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D197" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="E193" s="3">
-        <v>0</v>
-      </c>
-      <c r="F193" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D194" s="3" t="s">
+      <c r="E197" s="3">
+        <v>0</v>
+      </c>
+      <c r="F197" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D198" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="E194" s="3">
-        <v>0</v>
-      </c>
-      <c r="F194" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D195" s="3" t="s">
+      <c r="E198" s="3">
+        <v>0</v>
+      </c>
+      <c r="F198" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D199" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="E195" s="3">
-        <v>0</v>
-      </c>
-      <c r="F195" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D196" s="3" t="s">
+      <c r="E199" s="3">
+        <v>0</v>
+      </c>
+      <c r="F199" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D200" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="E196" s="3">
-        <v>0</v>
-      </c>
-      <c r="F196" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A197" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B197" s="3">
+      <c r="E200" s="3">
+        <v>0</v>
+      </c>
+      <c r="F200" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A201" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B201" s="3">
         <v>2898</v>
       </c>
-      <c r="C197" s="3">
+      <c r="C201" s="3">
         <v>22</v>
       </c>
-      <c r="D197" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E197" s="3">
+      <c r="D201" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E201" s="3">
         <v>185</v>
       </c>
-      <c r="F197" s="3">
+      <c r="F201" s="3">
         <v>2</v>
       </c>
-      <c r="G197" s="3">
+      <c r="G201" s="3">
         <v>6.0006487187804094</v>
       </c>
-      <c r="H197" s="3">
+      <c r="H201" s="3">
         <v>8.3333333333333321</v>
       </c>
     </row>
-    <row r="199" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A199" s="3" t="s">
+    <row r="203" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A203" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="B199" s="3">
+      <c r="B203" s="3">
         <v>11</v>
       </c>
-      <c r="C199" s="3">
+      <c r="C203" s="3">
         <v>463</v>
       </c>
-      <c r="D199" s="3" t="s">
+      <c r="D203" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="E199" s="3">
-        <v>0</v>
-      </c>
-      <c r="F199" s="3">
+      <c r="E203" s="3">
+        <v>0</v>
+      </c>
+      <c r="F203" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A200" s="3" t="s">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A204" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="B200" s="3">
-        <v>0</v>
-      </c>
-      <c r="C200" s="3">
+      <c r="B204" s="3">
+        <v>0</v>
+      </c>
+      <c r="C204" s="3">
         <v>3</v>
       </c>
-      <c r="D200" s="3" t="s">
+      <c r="D204" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="E200" s="3">
-        <v>0</v>
-      </c>
-      <c r="F200" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D201" s="3" t="s">
+      <c r="E204" s="3">
+        <v>0</v>
+      </c>
+      <c r="F204" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D205" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="E201" s="3">
-        <v>0</v>
-      </c>
-      <c r="F201" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A202" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B202" s="3">
-        <v>11</v>
-      </c>
-      <c r="C202" s="3">
-        <v>466</v>
-      </c>
-      <c r="D202" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E202" s="3">
-        <v>0</v>
-      </c>
-      <c r="F202" s="3">
-        <v>4</v>
-      </c>
-      <c r="G202" s="3">
-        <v>0</v>
-      </c>
-      <c r="H202" s="3">
-        <v>0.85106382978723405</v>
-      </c>
-    </row>
-    <row r="204" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A204" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="B204" s="3">
-        <v>829</v>
-      </c>
-      <c r="C204" s="3">
-        <v>480</v>
-      </c>
-      <c r="D204" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="E204" s="3">
-        <v>487</v>
-      </c>
-      <c r="F204" s="3">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="205" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A205" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="B205" s="3">
-        <v>486</v>
-      </c>
-      <c r="C205" s="3">
-        <v>18</v>
-      </c>
-      <c r="D205" s="3" t="s">
-        <v>238</v>
-      </c>
       <c r="E205" s="3">
-        <v>1473</v>
+        <v>0</v>
       </c>
       <c r="F205" s="3">
-        <v>36</v>
+        <v>0</v>
       </c>
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.25">
@@ -4425,26 +4429,32 @@
         <v>13</v>
       </c>
       <c r="B206" s="3">
-        <v>1315</v>
+        <v>11</v>
       </c>
       <c r="C206" s="3">
-        <v>498</v>
+        <v>466</v>
       </c>
       <c r="D206" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E206" s="3">
-        <v>1960</v>
+        <v>0</v>
       </c>
       <c r="F206" s="3">
-        <v>355</v>
+        <v>4</v>
       </c>
       <c r="G206" s="3">
-        <v>59.847328244274813</v>
+        <v>0</v>
       </c>
       <c r="H206" s="3">
-        <v>41.617819460726849</v>
-      </c>
+        <v>0.85106382978723405</v>
+      </c>
+    </row>
+    <row r="208" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="209" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A210" s="6"/>
+      <c r="D210" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>